<commit_message>
Enhance playoff and pool creation logic with match winners support; update tests accordingly
</commit_message>
<xml_diff>
--- a/pools-example-medium.xlsx
+++ b/pools-example-medium.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Elimination Round 1</t>
   </si>
@@ -318,54 +318,6 @@
   </si>
   <si>
     <t>YGRITTE</t>
-  </si>
-  <si>
-    <t>Pool A.1</t>
-  </si>
-  <si>
-    <t>Pool B.2</t>
-  </si>
-  <si>
-    <t>Pool C.1</t>
-  </si>
-  <si>
-    <t>Pool D.2</t>
-  </si>
-  <si>
-    <t>Pool E.1</t>
-  </si>
-  <si>
-    <t>Pool F.2</t>
-  </si>
-  <si>
-    <t>Pool G.1</t>
-  </si>
-  <si>
-    <t>Pool H.2</t>
-  </si>
-  <si>
-    <t>Pool B.1</t>
-  </si>
-  <si>
-    <t>Pool A.2</t>
-  </si>
-  <si>
-    <t>Pool D.1</t>
-  </si>
-  <si>
-    <t>Pool C.2</t>
-  </si>
-  <si>
-    <t>Pool F.1</t>
-  </si>
-  <si>
-    <t>Pool E.2</t>
-  </si>
-  <si>
-    <t>Pool H.1</t>
-  </si>
-  <si>
-    <t>Pool G.2</t>
   </si>
   <si>
     <t>Red</t>
@@ -535,12 +487,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="1"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -551,6 +497,12 @@
       <b val="1"/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -650,6 +602,39 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
     </border>
     <border>
       <left style="medium">
@@ -663,11 +648,6 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="medium">
@@ -696,34 +676,6 @@
         <color rgb="FF000000"/>
       </right>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -778,115 +730,115 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="false">
-      <alignment/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="false">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2518,360 +2470,360 @@
   <sheetData>
     <row r="1"/>
     <row r="2">
-      <c r="A2" s="25" t="str">
+      <c r="A2" s="36" t="str">
         <f>data!$A$4</f>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>92</v>
+      <c r="C2" s="35" t="str">
+        <f>CONCATENATE("Pool A.1",'Pool Matches'!G10)</f>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="26" t="str">
+      <c r="A3" s="37" t="str">
         <f>data!$B$2</f>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21">
+      <c r="D3" s="34"/>
+      <c r="E3" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="27" t="str">
+      <c r="A4" s="38" t="str">
         <f>data!$B$3</f>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="20"/>
+      <c r="C4" s="35" t="str">
+        <f>CONCATENATE("Pool B.2",'Pool Matches'!O11)</f>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5">
-      <c r="A5" s="28" t="str">
+      <c r="A5" s="39" t="str">
         <f>data!$B$4</f>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="33">
         <v>9</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="22"/>
-      <c r="C6" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="20"/>
+      <c r="A6" s="34"/>
+      <c r="C6" s="35" t="str">
+        <f>CONCATENATE("Pool C.1",'Pool Matches'!G21)</f>
+      </c>
+      <c r="G6" s="32"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7">
-      <c r="A7" s="25" t="str">
+      <c r="A7" s="36" t="str">
         <f>data!$A$7</f>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="21">
+      <c r="D7" s="34"/>
+      <c r="E7" s="33">
         <v>2</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="32"/>
+      <c r="I7" s="32"/>
     </row>
     <row r="8">
-      <c r="A8" s="26" t="str">
+      <c r="A8" s="37" t="str">
         <f>data!$B$5</f>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="20"/>
-      <c r="I8" s="20"/>
+      <c r="C8" s="35" t="str">
+        <f>CONCATENATE("Pool D.2",'Pool Matches'!O22)</f>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="32"/>
+      <c r="I8" s="32"/>
     </row>
     <row r="9">
-      <c r="A9" s="27" t="str">
+      <c r="A9" s="38" t="str">
         <f>data!$B$6</f>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="33">
         <v>13</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="28" t="str">
+      <c r="A10" s="39" t="str">
         <f>data!$B$7</f>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="20"/>
+      <c r="C10" s="35" t="str">
+        <f>CONCATENATE("Pool E.1",'Pool Matches'!G32)</f>
+      </c>
+      <c r="I10" s="32"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="32"/>
     </row>
     <row r="11">
-      <c r="A11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="21">
+      <c r="A11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="33">
         <v>3</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="I11" s="32"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12">
-      <c r="A12" s="25" t="str">
+      <c r="A12" s="36" t="str">
         <f>data!$A$10</f>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="K12" s="20"/>
+      <c r="C12" s="35" t="str">
+        <f>CONCATENATE("Pool F.2",'Pool Matches'!O33)</f>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="K12" s="32"/>
     </row>
     <row r="13">
-      <c r="A13" s="26" t="str">
+      <c r="A13" s="37" t="str">
         <f>data!$B$8</f>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="33">
         <v>10</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="20"/>
-      <c r="K13" s="20"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="32"/>
+      <c r="K13" s="32"/>
     </row>
     <row r="14">
-      <c r="A14" s="27" t="str">
+      <c r="A14" s="38" t="str">
         <f>data!$B$9</f>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G14" s="20"/>
-      <c r="K14" s="20"/>
+      <c r="C14" s="35" t="str">
+        <f>CONCATENATE("Pool G.1",'Pool Matches'!G43)</f>
+      </c>
+      <c r="G14" s="32"/>
+      <c r="K14" s="32"/>
     </row>
     <row r="15">
-      <c r="A15" s="28" t="str">
+      <c r="A15" s="39" t="str">
         <f>data!$B$10</f>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="21">
+      <c r="D15" s="34"/>
+      <c r="E15" s="33">
         <v>4</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="20"/>
-      <c r="K15" s="20"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="32"/>
+      <c r="K15" s="32"/>
     </row>
     <row r="16">
-      <c r="A16" s="22"/>
-      <c r="C16" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="20"/>
-      <c r="K16" s="20"/>
+      <c r="A16" s="34"/>
+      <c r="C16" s="35" t="str">
+        <f>CONCATENATE("Pool H.2",'Pool Matches'!O44)</f>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="32"/>
+      <c r="K16" s="32"/>
     </row>
     <row r="17">
-      <c r="A17" s="25" t="str">
+      <c r="A17" s="36" t="str">
         <f>data!$A$13</f>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="33">
         <v>15</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="26" t="str">
+      <c r="A18" s="37" t="str">
         <f>data!$B$11</f>
       </c>
-      <c r="C18" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K18" s="20"/>
+      <c r="C18" s="35" t="str">
+        <f>CONCATENATE("Pool B.1",'Pool Matches'!O10)</f>
+      </c>
+      <c r="K18" s="32"/>
     </row>
     <row r="19">
-      <c r="A19" s="27" t="str">
+      <c r="A19" s="38" t="str">
         <f>data!$B$12</f>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="21">
+      <c r="D19" s="34"/>
+      <c r="E19" s="33">
         <v>5</v>
       </c>
-      <c r="K19" s="20"/>
+      <c r="K19" s="32"/>
     </row>
     <row r="20">
-      <c r="A20" s="28" t="str">
+      <c r="A20" s="39" t="str">
         <f>data!$B$13</f>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="20"/>
-      <c r="K20" s="20"/>
+      <c r="C20" s="35" t="str">
+        <f>CONCATENATE("Pool A.2",'Pool Matches'!G11)</f>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="32"/>
+      <c r="K20" s="32"/>
     </row>
     <row r="21">
-      <c r="A21" s="22"/>
-      <c r="G21" s="21">
+      <c r="A21" s="34"/>
+      <c r="G21" s="33">
         <v>11</v>
       </c>
-      <c r="K21" s="20"/>
+      <c r="K21" s="32"/>
     </row>
     <row r="22">
-      <c r="A22" s="25" t="str">
+      <c r="A22" s="36" t="str">
         <f>data!$A$16</f>
       </c>
-      <c r="C22" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="C22" s="35" t="str">
+        <f>CONCATENATE("Pool D.1",'Pool Matches'!O21)</f>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="32"/>
+      <c r="K22" s="32"/>
     </row>
     <row r="23">
-      <c r="A23" s="26" t="str">
+      <c r="A23" s="37" t="str">
         <f>data!$B$14</f>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="21">
+      <c r="D23" s="34"/>
+      <c r="E23" s="33">
         <v>6</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="K23" s="32"/>
     </row>
     <row r="24">
-      <c r="A24" s="27" t="str">
+      <c r="A24" s="38" t="str">
         <f>data!$B$15</f>
       </c>
-      <c r="C24" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="K24" s="20"/>
+      <c r="C24" s="35" t="str">
+        <f>CONCATENATE("Pool C.2",'Pool Matches'!G22)</f>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="K24" s="32"/>
     </row>
     <row r="25">
-      <c r="A25" s="28" t="str">
+      <c r="A25" s="39" t="str">
         <f>data!$B$16</f>
       </c>
-      <c r="I25" s="21">
+      <c r="I25" s="33">
         <v>14</v>
       </c>
-      <c r="J25" s="23"/>
-      <c r="K25" s="20"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="32"/>
     </row>
     <row r="26">
-      <c r="A26" s="22"/>
-      <c r="C26" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="I26" s="20"/>
+      <c r="A26" s="34"/>
+      <c r="C26" s="35" t="str">
+        <f>CONCATENATE("Pool F.1",'Pool Matches'!O32)</f>
+      </c>
+      <c r="I26" s="32"/>
     </row>
     <row r="27">
-      <c r="A27" s="25" t="str">
+      <c r="A27" s="36" t="str">
         <f>data!$A$19</f>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="21">
+      <c r="D27" s="34"/>
+      <c r="E27" s="33">
         <v>7</v>
       </c>
-      <c r="I27" s="20"/>
+      <c r="I27" s="32"/>
     </row>
     <row r="28">
-      <c r="A28" s="26" t="str">
+      <c r="A28" s="37" t="str">
         <f>data!$B$17</f>
       </c>
-      <c r="C28" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="20"/>
-      <c r="I28" s="20"/>
+      <c r="C28" s="35" t="str">
+        <f>CONCATENATE("Pool E.2",'Pool Matches'!G33)</f>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="32"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29">
-      <c r="A29" s="27" t="str">
+      <c r="A29" s="38" t="str">
         <f>data!$B$18</f>
       </c>
-      <c r="G29" s="21">
+      <c r="G29" s="33">
         <v>12</v>
       </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="20"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="32"/>
     </row>
     <row r="30">
-      <c r="A30" s="28" t="str">
+      <c r="A30" s="39" t="str">
         <f>data!$B$19</f>
       </c>
-      <c r="C30" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="G30" s="20"/>
+      <c r="C30" s="35" t="str">
+        <f>CONCATENATE("Pool H.1",'Pool Matches'!O43)</f>
+      </c>
+      <c r="G30" s="32"/>
     </row>
     <row r="31">
-      <c r="A31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="21">
+      <c r="A31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="33">
         <v>8</v>
       </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="20"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32">
-      <c r="A32" s="25" t="str">
+      <c r="A32" s="36" t="str">
         <f>data!$A$22</f>
       </c>
-      <c r="C32" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="20"/>
+      <c r="C32" s="35" t="str">
+        <f>CONCATENATE("Pool G.2",'Pool Matches'!G44)</f>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="32"/>
     </row>
     <row r="33">
-      <c r="A33" s="26" t="str">
+      <c r="A33" s="37" t="str">
         <f>data!$B$20</f>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="27" t="str">
+      <c r="A34" s="38" t="str">
         <f>data!$B$21</f>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="str">
+      <c r="A35" s="39" t="str">
         <f>data!$B$22</f>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="22"/>
+      <c r="A36" s="34"/>
     </row>
     <row r="37">
-      <c r="A37" s="25" t="str">
+      <c r="A37" s="36" t="str">
         <f>data!$A$25</f>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="26" t="str">
+      <c r="A38" s="37" t="str">
         <f>data!$B$23</f>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="27" t="str">
+      <c r="A39" s="38" t="str">
         <f>data!$B$24</f>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="str">
+      <c r="A40" s="39" t="str">
         <f>data!$B$25</f>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="22"/>
+      <c r="A41" s="34"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
@@ -3313,582 +3265,582 @@
     <row r="2"/>
     <row r="3"/>
     <row r="4">
-      <c r="A4" s="29" t="str">
+      <c r="A4" s="20" t="str">
         <f>data!$A$4</f>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="I4" s="29" t="str">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="I4" s="20" t="str">
         <f>data!$A$7</f>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
     </row>
     <row r="5">
-      <c r="A5" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L5" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="O5" s="33" t="s">
-        <v>110</v>
+      <c r="A5" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="31" t="str">
+      <c r="A6" s="22" t="str">
         <f>data!$B$2</f>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31" t="str">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22" t="str">
         <f>data!$B$3</f>
       </c>
-      <c r="I6" s="31" t="str">
+      <c r="I6" s="22" t="str">
         <f>data!$B$5</f>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31" t="str">
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22" t="str">
         <f>data!$B$6</f>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="31" t="str">
+      <c r="A7" s="22" t="str">
         <f>data!$B$4</f>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31" t="str">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22" t="str">
         <f>data!$B$3</f>
       </c>
-      <c r="I7" s="31" t="str">
+      <c r="I7" s="22" t="str">
         <f>data!$B$7</f>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31" t="str">
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22" t="str">
         <f>data!$B$6</f>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="31" t="str">
+      <c r="A8" s="22" t="str">
         <f>data!$B$4</f>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31" t="str">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22" t="str">
         <f>data!$B$2</f>
       </c>
-      <c r="I8" s="31" t="str">
+      <c r="I8" s="22" t="str">
         <f>data!$B$7</f>
       </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31" t="str">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22" t="str">
         <f>data!$B$5</f>
       </c>
     </row>
     <row r="9"/>
     <row r="10">
       <c r="F10" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="G10" s="24"/>
       <c r="N10" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O10" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="O10" s="24"/>
     </row>
     <row r="11">
       <c r="F11" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G11" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="G11" s="24"/>
       <c r="N11" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="O11" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="O11" s="24"/>
     </row>
     <row r="12">
       <c r="F12" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G12" s="23"/>
+        <v>97</v>
+      </c>
+      <c r="G12" s="24"/>
       <c r="N12" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="O12" s="23"/>
+        <v>97</v>
+      </c>
+      <c r="O12" s="24"/>
     </row>
     <row r="13"/>
     <row r="14"/>
     <row r="15">
-      <c r="A15" s="29" t="str">
+      <c r="A15" s="20" t="str">
         <f>data!$A$10</f>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="I15" s="29" t="str">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="I15" s="20" t="str">
         <f>data!$A$13</f>
       </c>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
     </row>
     <row r="16">
-      <c r="A16" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="I16" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L16" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="O16" s="35" t="s">
-        <v>110</v>
+      <c r="A16" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L16" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="O16" s="27" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="31" t="str">
+      <c r="A17" s="22" t="str">
         <f>data!$B$8</f>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31" t="str">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22" t="str">
         <f>data!$B$9</f>
       </c>
-      <c r="I17" s="31" t="str">
+      <c r="I17" s="22" t="str">
         <f>data!$B$11</f>
       </c>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31" t="str">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22" t="str">
         <f>data!$B$12</f>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="31" t="str">
+      <c r="A18" s="22" t="str">
         <f>data!$B$10</f>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31" t="str">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22" t="str">
         <f>data!$B$9</f>
       </c>
-      <c r="I18" s="31" t="str">
+      <c r="I18" s="22" t="str">
         <f>data!$B$13</f>
       </c>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31" t="str">
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22" t="str">
         <f>data!$B$12</f>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="31" t="str">
+      <c r="A19" s="22" t="str">
         <f>data!$B$10</f>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31" t="str">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22" t="str">
         <f>data!$B$8</f>
       </c>
-      <c r="I19" s="31" t="str">
+      <c r="I19" s="22" t="str">
         <f>data!$B$13</f>
       </c>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31" t="str">
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22" t="str">
         <f>data!$B$11</f>
       </c>
     </row>
     <row r="20"/>
     <row r="21">
       <c r="F21" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="G21" s="24"/>
       <c r="N21" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O21" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="O21" s="24"/>
     </row>
     <row r="22">
       <c r="F22" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G22" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="G22" s="24"/>
       <c r="N22" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="O22" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="O22" s="24"/>
     </row>
     <row r="23">
       <c r="F23" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G23" s="23"/>
+        <v>97</v>
+      </c>
+      <c r="G23" s="24"/>
       <c r="N23" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="O23" s="23"/>
+        <v>97</v>
+      </c>
+      <c r="O23" s="24"/>
     </row>
     <row r="24"/>
     <row r="25"/>
     <row r="26">
-      <c r="A26" s="29" t="str">
+      <c r="A26" s="20" t="str">
         <f>data!$A$16</f>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="I26" s="29" t="str">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="I26" s="20" t="str">
         <f>data!$A$19</f>
       </c>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="29"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
     </row>
     <row r="27">
-      <c r="A27" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="G27" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="I27" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L27" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="O27" s="37" t="s">
-        <v>110</v>
+      <c r="A27" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="O27" s="29" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="31" t="str">
+      <c r="A28" s="22" t="str">
         <f>data!$B$14</f>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31" t="str">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22" t="str">
         <f>data!$B$15</f>
       </c>
-      <c r="I28" s="31" t="str">
+      <c r="I28" s="22" t="str">
         <f>data!$B$17</f>
       </c>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31" t="str">
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22" t="str">
         <f>data!$B$18</f>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="31" t="str">
+      <c r="A29" s="22" t="str">
         <f>data!$B$16</f>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31" t="str">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22" t="str">
         <f>data!$B$15</f>
       </c>
-      <c r="I29" s="31" t="str">
+      <c r="I29" s="22" t="str">
         <f>data!$B$19</f>
       </c>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31" t="str">
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22" t="str">
         <f>data!$B$18</f>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="31" t="str">
+      <c r="A30" s="22" t="str">
         <f>data!$B$16</f>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31" t="str">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22" t="str">
         <f>data!$B$14</f>
       </c>
-      <c r="I30" s="31" t="str">
+      <c r="I30" s="22" t="str">
         <f>data!$B$19</f>
       </c>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31" t="str">
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22" t="str">
         <f>data!$B$17</f>
       </c>
     </row>
     <row r="31"/>
     <row r="32">
       <c r="F32" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G32" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="G32" s="24"/>
       <c r="N32" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O32" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="O32" s="24"/>
     </row>
     <row r="33">
       <c r="F33" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G33" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="G33" s="24"/>
       <c r="N33" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="O33" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="O33" s="24"/>
     </row>
     <row r="34">
       <c r="F34" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G34" s="23"/>
+        <v>97</v>
+      </c>
+      <c r="G34" s="24"/>
       <c r="N34" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="O34" s="23"/>
+        <v>97</v>
+      </c>
+      <c r="O34" s="24"/>
     </row>
     <row r="35"/>
     <row r="36"/>
     <row r="37">
-      <c r="A37" s="29" t="str">
+      <c r="A37" s="20" t="str">
         <f>data!$A$22</f>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="I37" s="29" t="str">
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="I37" s="20" t="str">
         <f>data!$A$25</f>
       </c>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
     </row>
     <row r="38">
-      <c r="A38" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="G38" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="I38" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L38" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="O38" s="39" t="s">
-        <v>110</v>
+      <c r="A38" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L38" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="O38" s="31" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="31" t="str">
+      <c r="A39" s="22" t="str">
         <f>data!$B$20</f>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31" t="str">
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22" t="str">
         <f>data!$B$21</f>
       </c>
-      <c r="I39" s="31" t="str">
+      <c r="I39" s="22" t="str">
         <f>data!$B$23</f>
       </c>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="31"/>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31" t="str">
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22" t="str">
         <f>data!$B$24</f>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="31" t="str">
+      <c r="A40" s="22" t="str">
         <f>data!$B$22</f>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31" t="str">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22" t="str">
         <f>data!$B$21</f>
       </c>
-      <c r="I40" s="31" t="str">
+      <c r="I40" s="22" t="str">
         <f>data!$B$25</f>
       </c>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31" t="str">
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="22" t="str">
         <f>data!$B$24</f>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="31" t="str">
+      <c r="A41" s="22" t="str">
         <f>data!$B$22</f>
       </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31" t="str">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22" t="str">
         <f>data!$B$20</f>
       </c>
-      <c r="I41" s="31" t="str">
+      <c r="I41" s="22" t="str">
         <f>data!$B$25</f>
       </c>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31" t="str">
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="22"/>
+      <c r="N41" s="22"/>
+      <c r="O41" s="22" t="str">
         <f>data!$B$23</f>
       </c>
     </row>
     <row r="42"/>
     <row r="43">
       <c r="F43" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G43" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="G43" s="24"/>
       <c r="N43" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O43" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="O43" s="24"/>
     </row>
     <row r="44">
       <c r="F44" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G44" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="G44" s="24"/>
       <c r="N44" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="O44" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="O44" s="24"/>
     </row>
     <row r="45">
       <c r="F45" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G45" s="23"/>
+        <v>97</v>
+      </c>
+      <c r="G45" s="24"/>
       <c r="N45" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="O45" s="23"/>
+        <v>97</v>
+      </c>
+      <c r="O45" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3930,370 +3882,370 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="true">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2"/>
     <row r="3">
-      <c r="A3" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="I3" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
+      <c r="A3" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="I3" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
     </row>
     <row r="4">
-      <c r="A4" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>109</v>
+      <c r="A4" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L4" s="31" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="O4" s="43" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="31" t="str">
+      <c r="A5" s="22" t="str">
         <f>CONCATENATE("Pool A.1 ",'Pool Matches'!G10)</f>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31" t="str">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22" t="str">
         <f>CONCATENATE("Pool B.2 ",'Pool Matches'!O11)</f>
       </c>
-      <c r="I5" s="31" t="str">
+      <c r="I5" s="22" t="str">
         <f>CONCATENATE("Pool C.1 ",'Pool Matches'!G21)</f>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31" t="str">
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22" t="str">
         <f>CONCATENATE("Pool D.2 ",'Pool Matches'!O22)</f>
       </c>
     </row>
     <row r="6"/>
     <row r="7">
       <c r="F7" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G7" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="G7" s="24"/>
       <c r="N7" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="O7" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="O7" s="24"/>
     </row>
     <row r="8">
       <c r="F8" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G8" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="G8" s="24"/>
       <c r="N8" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="O8" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="O8" s="24"/>
     </row>
     <row r="9"/>
     <row r="10"/>
     <row r="11">
-      <c r="A11" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="I11" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
+      <c r="A11" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="I11" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
     </row>
     <row r="12">
-      <c r="A12" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>109</v>
+      <c r="A12" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L12" s="31" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="O12" s="45" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="31" t="str">
+      <c r="A13" s="22" t="str">
         <f>CONCATENATE("Pool E.1 ",'Pool Matches'!G32)</f>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="str">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22" t="str">
         <f>CONCATENATE("Pool F.2 ",'Pool Matches'!O33)</f>
       </c>
-      <c r="I13" s="31" t="str">
+      <c r="I13" s="22" t="str">
         <f>CONCATENATE("Pool G.1 ",'Pool Matches'!G43)</f>
       </c>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31" t="str">
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22" t="str">
         <f>CONCATENATE("Pool H.2 ",'Pool Matches'!O44)</f>
       </c>
     </row>
     <row r="14"/>
     <row r="15">
       <c r="F15" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G15" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="G15" s="24"/>
       <c r="N15" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="O15" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="O15" s="24"/>
     </row>
     <row r="16">
       <c r="F16" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="G16" s="24"/>
       <c r="N16" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="O16" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="O16" s="24"/>
     </row>
     <row r="17"/>
     <row r="18"/>
     <row r="19">
-      <c r="A19" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="I19" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
+      <c r="A19" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="I19" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
     </row>
     <row r="20">
-      <c r="A20" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>109</v>
+      <c r="A20" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="G20" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L20" s="31" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="O20" s="47" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="31" t="str">
+      <c r="A21" s="22" t="str">
         <f>CONCATENATE("Pool B.1 ",'Pool Matches'!O10)</f>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31" t="str">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22" t="str">
         <f>CONCATENATE("Pool A.2 ",'Pool Matches'!G11)</f>
       </c>
-      <c r="I21" s="31" t="str">
+      <c r="I21" s="22" t="str">
         <f>CONCATENATE("Pool D.1 ",'Pool Matches'!O21)</f>
       </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31" t="str">
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22" t="str">
         <f>CONCATENATE("Pool C.2 ",'Pool Matches'!G22)</f>
       </c>
     </row>
     <row r="22"/>
     <row r="23">
       <c r="F23" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G23" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="G23" s="24"/>
       <c r="N23" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="O23" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="O23" s="24"/>
     </row>
     <row r="24">
       <c r="F24" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G24" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="G24" s="24"/>
       <c r="N24" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="O24" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="O24" s="24"/>
     </row>
     <row r="25"/>
     <row r="26"/>
     <row r="27">
-      <c r="A27" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="I27" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
+      <c r="A27" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="I27" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
     </row>
     <row r="28">
-      <c r="A28" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>109</v>
+      <c r="A28" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="G28" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="I28" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L28" s="31" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L28" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="O28" s="49" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="31" t="str">
+      <c r="A29" s="22" t="str">
         <f>CONCATENATE("Pool F.1 ",'Pool Matches'!O32)</f>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31" t="str">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22" t="str">
         <f>CONCATENATE("Pool E.2 ",'Pool Matches'!G33)</f>
       </c>
-      <c r="I29" s="31" t="str">
+      <c r="I29" s="22" t="str">
         <f>CONCATENATE("Pool H.1 ",'Pool Matches'!O43)</f>
       </c>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31" t="str">
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22" t="str">
         <f>CONCATENATE("Pool G.2 ",'Pool Matches'!G44)</f>
       </c>
     </row>
     <row r="30"/>
     <row r="31">
       <c r="F31" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G31" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="G31" s="24"/>
       <c r="N31" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="O31" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="O31" s="24"/>
     </row>
     <row r="32">
       <c r="F32" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G32" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="G32" s="24"/>
       <c r="N32" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="O32" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="O32" s="24"/>
     </row>
     <row r="33"/>
     <row r="34"/>
@@ -4303,196 +4255,196 @@
     <row r="38"/>
     <row r="39"/>
     <row r="40">
-      <c r="A40" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
+      <c r="A40" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
     </row>
     <row r="41"/>
     <row r="42">
-      <c r="A42" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="I42" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
+      <c r="A42" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="I42" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
     </row>
     <row r="43">
-      <c r="A43" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" s="31" t="s">
-        <v>109</v>
+      <c r="A43" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="G43" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="I43" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L43" s="31" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="I43" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L43" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="O43" s="51" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="31" t="str">
+      <c r="A44" s="22" t="str">
         <f>CONCATENATE("M 1 ",'Elimination Matches'!G7)</f>
       </c>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31" t="str">
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22" t="str">
         <f>CONCATENATE("M 2 ",'Elimination Matches'!O7)</f>
       </c>
-      <c r="I44" s="31" t="str">
+      <c r="I44" s="22" t="str">
         <f>CONCATENATE("M 3 ",'Elimination Matches'!G15)</f>
       </c>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="31"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="31"/>
-      <c r="O44" s="31" t="str">
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="22" t="str">
         <f>CONCATENATE("M 4 ",'Elimination Matches'!O15)</f>
       </c>
     </row>
     <row r="45"/>
     <row r="46">
       <c r="F46" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G46" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="G46" s="24"/>
       <c r="N46" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="O46" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="O46" s="24"/>
     </row>
     <row r="47">
       <c r="F47" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G47" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="G47" s="24"/>
       <c r="N47" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="O47" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="O47" s="24"/>
     </row>
     <row r="48"/>
     <row r="49"/>
     <row r="50">
-      <c r="A50" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="I50" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="29"/>
+      <c r="A50" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="I50" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="20"/>
     </row>
     <row r="51">
-      <c r="A51" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>109</v>
+      <c r="A51" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="G51" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="I51" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L51" s="31" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="I51" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L51" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="O51" s="53" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="31" t="str">
+      <c r="A52" s="22" t="str">
         <f>CONCATENATE("M 5 ",'Elimination Matches'!G23)</f>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31" t="str">
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22" t="str">
         <f>CONCATENATE("M 6 ",'Elimination Matches'!O23)</f>
       </c>
-      <c r="I52" s="31" t="str">
+      <c r="I52" s="22" t="str">
         <f>CONCATENATE("M 7 ",'Elimination Matches'!G31)</f>
       </c>
-      <c r="J52" s="31"/>
-      <c r="K52" s="31"/>
-      <c r="L52" s="31"/>
-      <c r="M52" s="31"/>
-      <c r="N52" s="31"/>
-      <c r="O52" s="31" t="str">
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="22"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22" t="str">
         <f>CONCATENATE("M 8 ",'Elimination Matches'!O31)</f>
       </c>
     </row>
     <row r="53"/>
     <row r="54">
       <c r="F54" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G54" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="G54" s="24"/>
       <c r="N54" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="O54" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="O54" s="24"/>
     </row>
     <row r="55">
       <c r="F55" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G55" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="G55" s="24"/>
       <c r="N55" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="O55" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="O55" s="24"/>
     </row>
     <row r="56"/>
     <row r="57"/>
@@ -4502,109 +4454,109 @@
     <row r="61"/>
     <row r="62"/>
     <row r="63">
-      <c r="A63" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="B63" s="29"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="29"/>
-      <c r="I63" s="29"/>
-      <c r="J63" s="29"/>
-      <c r="K63" s="29"/>
-      <c r="L63" s="29"/>
-      <c r="M63" s="29"/>
-      <c r="N63" s="29"/>
-      <c r="O63" s="29"/>
+      <c r="A63" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="20"/>
+      <c r="M63" s="20"/>
+      <c r="N63" s="20"/>
+      <c r="O63" s="20"/>
     </row>
     <row r="64"/>
     <row r="65">
-      <c r="A65" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="B65" s="29"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29"/>
-      <c r="I65" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="J65" s="29"/>
-      <c r="K65" s="29"/>
-      <c r="L65" s="29"/>
-      <c r="M65" s="29"/>
-      <c r="N65" s="29"/>
-      <c r="O65" s="29"/>
+      <c r="A65" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="I65" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="20"/>
+      <c r="M65" s="20"/>
+      <c r="N65" s="20"/>
+      <c r="O65" s="20"/>
     </row>
     <row r="66">
-      <c r="A66" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D66" s="31" t="s">
-        <v>109</v>
+      <c r="A66" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="G66" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="I66" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L66" s="31" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="I66" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L66" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="O66" s="55" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="31" t="str">
+      <c r="A67" s="22" t="str">
         <f>CONCATENATE("M 9 ",'Elimination Matches'!G46)</f>
       </c>
-      <c r="B67" s="31"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="31"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="31" t="str">
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22" t="str">
         <f>CONCATENATE("M 10 ",'Elimination Matches'!O46)</f>
       </c>
-      <c r="I67" s="31" t="str">
+      <c r="I67" s="22" t="str">
         <f>CONCATENATE("M 11 ",'Elimination Matches'!G54)</f>
       </c>
-      <c r="J67" s="31"/>
-      <c r="K67" s="31"/>
-      <c r="L67" s="31"/>
-      <c r="M67" s="31"/>
-      <c r="N67" s="31"/>
-      <c r="O67" s="31" t="str">
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
+      <c r="N67" s="22"/>
+      <c r="O67" s="22" t="str">
         <f>CONCATENATE("M 12 ",'Elimination Matches'!O54)</f>
       </c>
     </row>
     <row r="68"/>
     <row r="69">
       <c r="F69" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G69" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="G69" s="24"/>
       <c r="N69" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="O69" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="O69" s="24"/>
     </row>
     <row r="70">
       <c r="F70" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G70" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="G70" s="24"/>
       <c r="N70" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="O70" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="O70" s="24"/>
     </row>
     <row r="71"/>
     <row r="72"/>
@@ -4614,72 +4566,72 @@
     <row r="76"/>
     <row r="77"/>
     <row r="78">
-      <c r="A78" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="29"/>
-      <c r="I78" s="29"/>
-      <c r="J78" s="29"/>
-      <c r="K78" s="29"/>
-      <c r="L78" s="29"/>
-      <c r="M78" s="29"/>
-      <c r="N78" s="29"/>
-      <c r="O78" s="29"/>
+      <c r="A78" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B78" s="20"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
+      <c r="J78" s="20"/>
+      <c r="K78" s="20"/>
+      <c r="L78" s="20"/>
+      <c r="M78" s="20"/>
+      <c r="N78" s="20"/>
+      <c r="O78" s="20"/>
     </row>
     <row r="79"/>
     <row r="80">
-      <c r="A80" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B80" s="29"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="29"/>
-      <c r="G80" s="29"/>
+      <c r="A80" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
     </row>
     <row r="81">
-      <c r="A81" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D81" s="31" t="s">
-        <v>109</v>
+      <c r="A81" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D81" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="G81" s="56" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="31" t="str">
+      <c r="A82" s="22" t="str">
         <f>CONCATENATE("M 13 ",'Elimination Matches'!G69)</f>
       </c>
-      <c r="B82" s="31"/>
-      <c r="C82" s="31"/>
-      <c r="D82" s="31"/>
-      <c r="E82" s="31"/>
-      <c r="F82" s="31"/>
-      <c r="G82" s="31" t="str">
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22" t="str">
         <f>CONCATENATE("M 14 ",'Elimination Matches'!O69)</f>
       </c>
     </row>
     <row r="83"/>
     <row r="84">
       <c r="F84" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G84" s="23"/>
+        <v>99</v>
+      </c>
+      <c r="G84" s="24"/>
     </row>
     <row r="85">
       <c r="F85" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G85" s="23"/>
+        <v>100</v>
+      </c>
+      <c r="G85" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>